<commit_message>
New Test Cases created. One test performed
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160BCC48-8228-4DCC-AB6D-72C58F6B9056}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306E674D-AE20-4E95-93AB-A14519EE4B79}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="SEARCH_2_Return" sheetId="10" r:id="rId9"/>
     <sheet name="SEARCH_2_ReturNoDeparture" sheetId="11" r:id="rId10"/>
     <sheet name="SEARCH_2_ReturnNoDestination" sheetId="12" r:id="rId11"/>
-    <sheet name="SEARCH_2_ReturnNoDate" sheetId="9" r:id="rId12"/>
+    <sheet name="SEARCH_2_ReturnNoDepartureDate" sheetId="9" r:id="rId12"/>
+    <sheet name="SEARCH_2_ReturnNoArrivalDate" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="93">
   <si>
     <t>PROJECT</t>
   </si>
@@ -228,9 +229,6 @@
     <t>Error that no destination city has been selected or button will be disabled</t>
   </si>
   <si>
-    <t>Search for Flight from Wrocław</t>
-  </si>
-  <si>
     <t>SEARCH_1_OneWay</t>
   </si>
   <si>
@@ -279,10 +277,40 @@
     <t>SEARCH_2_Return</t>
   </si>
   <si>
-    <t>SEARCH_2_ReturnNoDate</t>
+    <t>Not yet tested</t>
   </si>
   <si>
-    <t>Not yet tested</t>
+    <t>SEARCH_2_ND</t>
+  </si>
+  <si>
+    <t>OneWayNoDate</t>
+  </si>
+  <si>
+    <t>Select one way flight, don't select date</t>
+  </si>
+  <si>
+    <t>Try to search for a flight with missing date</t>
+  </si>
+  <si>
+    <t>3.Provide London as destination</t>
+  </si>
+  <si>
+    <t>Error that no date has been selected and button will be disabled</t>
+  </si>
+  <si>
+    <t>4. Search flight</t>
+  </si>
+  <si>
+    <t>Flight button is inactive and information that no date has been selected occurs</t>
+  </si>
+  <si>
+    <t>SEARCH_2_ReturnNoDepartureDate</t>
+  </si>
+  <si>
+    <t>SEARCH_2_ReturnArrivaleDate</t>
+  </si>
+  <si>
+    <t>SEARCH_2_OneWayNoDate</t>
   </si>
 </sst>
 </file>
@@ -530,6 +558,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -548,15 +579,467 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Normalny 2" xfId="1" xr:uid="{197B7AA7-319A-4CB2-9511-8E2592BCCB12}"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="105">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1113,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD17"/>
+  <dimension ref="A1:XFD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,38 +1669,38 @@
         <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16384" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:16384" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16384" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
         <v>68</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -17631,7 +18114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16384" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
@@ -17659,18 +18142,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16384" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
@@ -17678,7 +18164,7 @@
         <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:16384" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17689,37 +18175,59 @@
         <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A6:A17">
-    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="zablokowany">
+  <conditionalFormatting sqref="A6:A19">
+    <cfRule type="containsText" dxfId="104" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",A6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="103" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",A6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="102" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",A6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="101" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A17">
-    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="negatywny">
+  <conditionalFormatting sqref="A6:A19">
+    <cfRule type="containsText" dxfId="100" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17730,38 +18238,676 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65647DFC-4D98-4C65-BD12-03FE5E4F7818}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:K1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7">
+        <v>43387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="49" priority="7" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="8" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="9" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="45" priority="6" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE7D7A9-6F73-4F6E-A6A0-310A2A52BF90}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:K1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7">
+        <v>43387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="39" priority="7" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="9" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="10" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D45DD5B-4563-4B70-B85B-34E6C3018917}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A7" sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7">
+        <v>43387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09D37E1-3F49-47A0-BBBC-FB16DF367D18}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:K1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7">
+        <v>43387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -17771,7 +18917,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17790,61 +18936,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="7">
         <v>43382</v>
       </c>
@@ -17921,7 +19067,7 @@
     </row>
     <row r="10" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>44</v>
@@ -17942,12 +19088,12 @@
         <v>46</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>53</v>
@@ -17968,12 +19114,12 @@
         <v>58</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>62</v>
@@ -17994,7 +19140,7 @@
         <v>64</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -18016,21 +19162,21 @@
     <mergeCell ref="A5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="99" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="98" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="97" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="96" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18042,7 +19188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE122FC-6A4F-472D-AFB4-3E463A66C1BD}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -18062,61 +19208,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="7">
         <v>43383</v>
       </c>
@@ -18217,7 +19363,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>52</v>
       </c>
@@ -18246,7 +19392,7 @@
         <v>21</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -18278,7 +19424,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -18291,21 +19437,21 @@
     <mergeCell ref="A5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="29" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="90" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18318,7 +19464,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A9" sqref="A9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18336,62 +19482,62 @@
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="7">
         <v>43383</v>
       </c>
@@ -18465,29 +19611,29 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="89" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="88" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="87" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="86" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18518,62 +19664,62 @@
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="7">
         <v>43383</v>
       </c>
@@ -18630,7 +19776,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -18644,44 +19790,44 @@
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="F10" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="F11" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F12" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="84" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="83" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="82" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="81" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="80" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18694,7 +19840,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A8" sqref="A8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18712,62 +19858,62 @@
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="7">
         <v>43383</v>
       </c>
@@ -18823,8 +19969,8 @@
       <c r="E9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>72</v>
+      <c r="F9" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>58</v>
@@ -18836,49 +19982,49 @@
         <v>21</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="F10" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="F11" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F12" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="79" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="78" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="77" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="76" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18891,7 +20037,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18909,62 +20055,62 @@
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="7">
         <v>43383</v>
       </c>
@@ -19021,7 +20167,7 @@
         <v>60</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>64</v>
@@ -19033,49 +20179,49 @@
         <v>21</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="74" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="70" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19085,10 +20231,225 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1201DBF-776F-4E80-B326-18F6F5DF3A00}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7">
+        <v>43387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F11" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="69" priority="7" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="8" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="9" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="10" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="65" priority="6" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="60" priority="1" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770724BE-A242-4B78-9330-98FF62807E0C}">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A7" sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19107,63 +20468,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="48" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="4" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="7">
-        <v>43383</v>
+        <v>43387</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -19210,37 +20571,44 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="zablokowany">
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="10" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="55" priority="6" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="54" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="52" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="51" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="negatywny">
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770724BE-A242-4B78-9330-98FF62807E0C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Return flights search functioanlity tested, Screenshots added
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306E674D-AE20-4E95-93AB-A14519EE4B79}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FAEB10-A546-45C4-8984-68FB604ADE06}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SEARCH_2_OneWayNoDestination" sheetId="7" r:id="rId7"/>
     <sheet name="SEARCH_2_OneWayNoDate" sheetId="8" r:id="rId8"/>
     <sheet name="SEARCH_2_Return" sheetId="10" r:id="rId9"/>
-    <sheet name="SEARCH_2_ReturNoDeparture" sheetId="11" r:id="rId10"/>
+    <sheet name="SEARCH_2_ReturnNoDeparture" sheetId="11" r:id="rId10"/>
     <sheet name="SEARCH_2_ReturnNoDestination" sheetId="12" r:id="rId11"/>
     <sheet name="SEARCH_2_ReturnNoDepartureDate" sheetId="9" r:id="rId12"/>
     <sheet name="SEARCH_2_ReturnNoArrivalDate" sheetId="13" r:id="rId13"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="126">
   <si>
     <t>PROJECT</t>
   </si>
@@ -277,9 +277,6 @@
     <t>SEARCH_2_Return</t>
   </si>
   <si>
-    <t>Not yet tested</t>
-  </si>
-  <si>
     <t>SEARCH_2_ND</t>
   </si>
   <si>
@@ -311,6 +308,108 @@
   </si>
   <si>
     <t>SEARCH_2_OneWayNoDate</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Select  One return flight</t>
+  </si>
+  <si>
+    <t>Test functionality of searching when option return ticket is selected</t>
+  </si>
+  <si>
+    <t>1. Select Return flight</t>
+  </si>
+  <si>
+    <t>2. Provide Wrocław as Departure and London as Destination</t>
+  </si>
+  <si>
+    <t>4.Select date of return</t>
+  </si>
+  <si>
+    <t>5.Click flight</t>
+  </si>
+  <si>
+    <t>Possible flights date from Wrocław to London on 9.11.2018 and possible flights from London to Wrocław on 11.11.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two possibe flights from Wrocław to London displayed and one possible flight from London to Wrocław </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Select return flight option </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flight button is inactive, It is impossible to select Date, information that no departure city has been selected </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proof that information occurs. Please check attachment: NoDepartureCity.png   </t>
+  </si>
+  <si>
+    <t>Try to search for a flight with missing destinantion city</t>
+  </si>
+  <si>
+    <t>2.  Provide Wrocław as Departure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flight button is inactive, It is impossible to select Date, information that no destination city has been selected </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proof that information occurs. Please check attachment: NoDestinationCity.png   </t>
+  </si>
+  <si>
+    <t>NoDepartureDate</t>
+  </si>
+  <si>
+    <t>Select return flight, don't select destination city.</t>
+  </si>
+  <si>
+    <t>Select return flight, don't select Departure city.</t>
+  </si>
+  <si>
+    <t>3. Provide London as destination</t>
+  </si>
+  <si>
+    <t>Error that no destinantion city has been selected or button will be disabled</t>
+  </si>
+  <si>
+    <t>Error that no departure date has been selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proof that information occurs. Please check attachment: NoDeparturenDate.png   </t>
+  </si>
+  <si>
+    <t>SEARCH_2_ReturnNoArrivalDate</t>
+  </si>
+  <si>
+    <t>NoArrivalDate</t>
+  </si>
+  <si>
+    <t>Select return flight, don't select date of Arrival</t>
+  </si>
+  <si>
+    <t>Try to search for a flight with missing departure date</t>
+  </si>
+  <si>
+    <t>Try to search for a flight with missing arrival date</t>
+  </si>
+  <si>
+    <t>4.Select date of departure</t>
+  </si>
+  <si>
+    <t>Error that no arrival date has been selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proof that information occurs. Please check attachment: NoArrivalnDate.png   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flight button is inactive, It is impossible to search, information that no arrival date has been selected occurs </t>
+  </si>
+  <si>
+    <t>Select return flight, don't select date of departure</t>
+  </si>
+  <si>
+    <t>Flight button is inactive, It is impossible to search, information that no departure date has been selected  occurs</t>
   </si>
 </sst>
 </file>
@@ -658,13 +757,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="2"/>
         </patternFill>
       </fill>
@@ -722,6 +814,13 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1599,7 +1698,7 @@
   <dimension ref="A1:XFD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18147,7 +18246,7 @@
         <v>49</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
         <v>43</v>
@@ -18164,7 +18263,10 @@
         <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:16384" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18175,10 +18277,13 @@
         <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
@@ -18186,29 +18291,38 @@
         <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -18238,10 +18352,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65647DFC-4D98-4C65-BD12-03FE5E4F7818}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:K1048576"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18254,12 +18368,12 @@
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
@@ -18269,7 +18383,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
@@ -18279,7 +18393,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
@@ -18289,7 +18403,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
@@ -18299,7 +18413,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
@@ -18316,7 +18430,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7">
-        <v>43387</v>
+        <v>43388</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -18354,14 +18468,66 @@
         <v>35</v>
       </c>
     </row>
+    <row r="9" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F10" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F11" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
     <cfRule type="containsText" dxfId="49" priority="7" operator="containsText" text="zablokowany">
@@ -18407,10 +18573,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE7D7A9-6F73-4F6E-A6A0-310A2A52BF90}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:K1048576"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18422,13 +18588,13 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
@@ -18438,7 +18604,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
@@ -18448,7 +18614,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
@@ -18458,7 +18624,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
@@ -18468,7 +18634,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
@@ -18485,7 +18651,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7">
-        <v>43387</v>
+        <v>43388</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -18523,50 +18689,102 @@
         <v>35</v>
       </c>
     </row>
+    <row r="9" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F10" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F11" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="39" priority="7" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="9" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="10" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18576,10 +18794,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D45DD5B-4563-4B70-B85B-34E6C3018917}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:K1048576"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18591,13 +18809,13 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
@@ -18607,7 +18825,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
@@ -18617,7 +18835,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
@@ -18627,7 +18845,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
@@ -18637,7 +18855,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
@@ -18654,7 +18872,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7">
-        <v>43387</v>
+        <v>43388</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -18692,14 +18910,66 @@
         <v>35</v>
       </c>
     </row>
+    <row r="9" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F10" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F11" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
     <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="zablokowany">
@@ -18745,10 +19015,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09D37E1-3F49-47A0-BBBC-FB16DF367D18}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:K1048576"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18761,12 +19031,12 @@
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
@@ -18776,7 +19046,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
@@ -18786,7 +19056,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
@@ -18796,7 +19066,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
@@ -18806,7 +19076,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
@@ -18823,7 +19093,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7">
-        <v>43387</v>
+        <v>43388</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -18861,50 +19131,102 @@
         <v>35</v>
       </c>
     </row>
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F10" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F11" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19646,7 +19968,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A9" sqref="A9:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19840,7 +20162,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:K8"/>
+      <selection activeCell="A9" sqref="A9:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20234,7 +20556,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A9" sqref="A9:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20347,30 +20669,30 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
         <v>82</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>43</v>
@@ -20385,12 +20707,12 @@
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="F11" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -20446,15 +20768,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770724BE-A242-4B78-9330-98FF62807E0C}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:K1048576"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
@@ -20462,12 +20784,12 @@
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
@@ -20477,7 +20799,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
@@ -20487,7 +20809,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
@@ -20497,7 +20819,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
@@ -20507,7 +20829,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
@@ -20524,7 +20846,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7">
-        <v>43387</v>
+        <v>43388</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -20562,14 +20884,63 @@
         <v>35</v>
       </c>
     </row>
+    <row r="9" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="F10" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F11" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
     <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="zablokowany">

</xml_diff>

<commit_message>
Files updated, Unnecessary screenshots removed
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FAEB10-A546-45C4-8984-68FB604ADE06}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8431ED-3E2B-456B-BBD5-87BD5AC1C8E8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="SEARCH1" sheetId="2" r:id="rId2"/>
-    <sheet name="SEARCH2" sheetId="3" r:id="rId3"/>
+    <sheet name="SEARCH1" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="SEARCH2" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="SEARCH_2_L" sheetId="4" r:id="rId4"/>
     <sheet name="SEARCH_2_OneWay" sheetId="5" r:id="rId5"/>
     <sheet name="SEARCH_2_OneWayNoDeparture" sheetId="6" r:id="rId6"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="129">
   <si>
     <t>PROJECT</t>
   </si>
@@ -343,9 +343,6 @@
     <t xml:space="preserve">Flight button is inactive, It is impossible to select Date, information that no departure city has been selected </t>
   </si>
   <si>
-    <t xml:space="preserve">Proof that information occurs. Please check attachment: NoDepartureCity.png   </t>
-  </si>
-  <si>
     <t>Try to search for a flight with missing destinantion city</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
   </si>
   <si>
     <t xml:space="preserve">Flight button is inactive, It is impossible to select Date, information that no destination city has been selected </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proof that information occurs. Please check attachment: NoDestinationCity.png   </t>
   </si>
   <si>
     <t>NoDepartureDate</t>
@@ -374,9 +368,6 @@
   </si>
   <si>
     <t>Error that no departure date has been selected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proof that information occurs. Please check attachment: NoDeparturenDate.png   </t>
   </si>
   <si>
     <t>SEARCH_2_ReturnNoArrivalDate</t>
@@ -400,9 +391,6 @@
     <t>Error that no arrival date has been selected</t>
   </si>
   <si>
-    <t xml:space="preserve">Proof that information occurs. Please check attachment: NoArrivalnDate.png   </t>
-  </si>
-  <si>
     <t xml:space="preserve">Flight button is inactive, It is impossible to search, information that no arrival date has been selected occurs </t>
   </si>
   <si>
@@ -410,6 +398,27 @@
   </si>
   <si>
     <t>Flight button is inactive, It is impossible to search, information that no departure date has been selected  occurs</t>
+  </si>
+  <si>
+    <t>Possible flights date from Wrocław to London on 9.11.2018 and possible flights from London to Wrocław on 11.11.2019</t>
+  </si>
+  <si>
+    <t>Possible flights date from Wrocław to London on 9.11.2018 and possible flights from London to Wrocław on 11.11.2020</t>
+  </si>
+  <si>
+    <t>Possible flights date from Wrocław to London on 9.11.2018 and possible flights from London to Wrocław on 11.11.2021</t>
+  </si>
+  <si>
+    <t>Possible flights date from Wrocław to London on 9.11.2018 and possible flights from London to Wrocław on 11.11.2022</t>
+  </si>
+  <si>
+    <t>Possible flights date from Wrocław to London on 9.11.2019</t>
+  </si>
+  <si>
+    <t>Possible flights date from Wrocław to London on 9.11.2020</t>
+  </si>
+  <si>
+    <t>Possible flights date from Wrocław to London on 9.11.2021</t>
   </si>
 </sst>
 </file>
@@ -683,77 +692,7 @@
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Normalny 2" xfId="1" xr:uid="{197B7AA7-319A-4CB2-9511-8E2592BCCB12}"/>
   </cellStyles>
-  <dxfs count="105">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="95">
     <dxf>
       <fill>
         <patternFill>
@@ -18327,21 +18266,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:A19">
-    <cfRule type="containsText" dxfId="104" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",A6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",A6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",A6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A19">
-    <cfRule type="containsText" dxfId="100" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="90" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18354,8 +18293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65647DFC-4D98-4C65-BD12-03FE5E4F7818}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18367,7 +18306,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -18468,7 +18407,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>79</v>
       </c>
@@ -18476,7 +18415,7 @@
         <v>53</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>42</v>
@@ -18496,28 +18435,62 @@
       <c r="J9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>103</v>
-      </c>
+      <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F10" s="9" t="s">
+    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="F10" s="10" t="s">
         <v>75</v>
       </c>
+      <c r="H10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F11" s="9" t="s">
+    <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="F11" s="10" t="s">
         <v>74</v>
       </c>
+      <c r="H11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+    <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="F12" s="10" t="s">
         <v>97</v>
       </c>
+      <c r="H12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
+    <row r="13" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="F13" s="10" t="s">
         <v>98</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -18530,40 +18503,40 @@
     <mergeCell ref="A5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="49" priority="7" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="39" priority="7" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="8" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="9" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="37" priority="9" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="36" priority="10" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="45" priority="6" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18576,7 +18549,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18588,7 +18561,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -18689,7 +18662,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>78</v>
       </c>
@@ -18697,269 +18670,82 @@
         <v>62</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>101</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>107</v>
-      </c>
+      <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F10" s="9" t="s">
+    <row r="10" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F10" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>105</v>
       </c>
+      <c r="J10" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F11" s="9" t="s">
+    <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F11" s="10" t="s">
         <v>74</v>
       </c>
+      <c r="H11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F12" s="10" t="s">
         <v>97</v>
       </c>
+      <c r="H12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
+    <row r="13" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F13" s="10" t="s">
         <v>98</v>
       </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-  </mergeCells>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="zablokowany">
-      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="pozytywny warunkowo">
-      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="pozytywny">
-      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="nieprzetestowano">
-      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="negatywny">
-      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="zablokowany">
-      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="pozytywny warunkowo">
-      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="pozytywny">
-      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="nieprzetestowano">
-      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="negatywny">
-      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D45DD5B-4563-4B70-B85B-34E6C3018917}">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="7">
-        <v>43388</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="H13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F10" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F11" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -19013,12 +18799,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09D37E1-3F49-47A0-BBBC-FB16DF367D18}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D45DD5B-4563-4B70-B85B-34E6C3018917}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19030,8 +18816,8 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -19131,56 +18917,344 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>101</v>
       </c>
       <c r="H9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>122</v>
-      </c>
+      <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F10" s="9" t="s">
-        <v>105</v>
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="F10" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F11" s="9" t="s">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="F11" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>111</v>
       </c>
+      <c r="I11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>120</v>
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="F12" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="F13" s="10" t="s">
         <v>98</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09D37E1-3F49-47A0-BBBC-FB16DF367D18}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="29.42578125" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7">
+        <v>43388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="F10" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="F11" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="F12" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="F13" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -19193,40 +19267,40 @@
     <mergeCell ref="A5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D5">
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19239,7 +19313,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19484,21 +19558,21 @@
     <mergeCell ref="A5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="99" priority="2" operator="containsText" text="zablokowany">
+    <cfRule type="containsText" dxfId="89" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="3" operator="containsText" text="pozytywny warunkowo">
+    <cfRule type="containsText" dxfId="88" priority="3" operator="containsText" text="pozytywny warunkowo">
       <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="4" operator="containsText" text="pozytywny">
+    <cfRule type="containsText" dxfId="87" priority="4" operator="containsText" text="pozytywny">
       <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="5" operator="containsText" text="nieprzetestowano">
+    <cfRule type="containsText" dxfId="86" priority="5" operator="containsText" text="nieprzetestowano">
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="negatywny">
+    <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19759,382 +19833,6 @@
     <mergeCell ref="A5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="zablokowany">
-      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="pozytywny warunkowo">
-      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="pozytywny">
-      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="nieprzetestowano">
-      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="90" priority="1" operator="containsText" text="negatywny">
-      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E88C7D-4FC7-4F65-839B-E8F149336215}">
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="7">
-        <v>43383</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-  </mergeCells>
-  <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="89" priority="2" operator="containsText" text="zablokowany">
-      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="3" operator="containsText" text="pozytywny warunkowo">
-      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="4" operator="containsText" text="pozytywny">
-      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="5" operator="containsText" text="nieprzetestowano">
-      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D6">
-    <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="negatywny">
-      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDAE7B8-F38F-4799-8D14-50737728AAB8}">
-  <dimension ref="A1:K12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:J12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="7">
-        <v>43383</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="F10" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F11" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-  </mergeCells>
-  <conditionalFormatting sqref="D1:D6">
     <cfRule type="containsText" dxfId="84" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
@@ -20157,24 +19855,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6FF35F-96E3-496A-B7B4-F19414F8B417}">
-  <dimension ref="A1:K12"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E88C7D-4FC7-4F65-839B-E8F149336215}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -20200,7 +19898,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
@@ -20210,7 +19908,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
@@ -20275,51 +19973,36 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>52</v>
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F10" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="F11" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" s="9" t="s">
-        <v>73</v>
+      <c r="J9" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -20354,25 +20037,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9741D50-4AEE-45D3-BFC6-BF01A15F6C84}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDAE7B8-F38F-4799-8D14-50737728AAB8}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -20397,7 +20080,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
@@ -20407,7 +20090,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
@@ -20472,51 +20155,75 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>63</v>
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>70</v>
+        <v>51</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>76</v>
+    <row r="10" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+    <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F11" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="H11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F12" s="6" t="s">
         <v>73</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -20551,27 +20258,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1201DBF-776F-4E80-B326-18F6F5DF3A00}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6FF35F-96E3-496A-B7B4-F19414F8B417}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:J12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -20631,7 +20338,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7">
-        <v>43387</v>
+        <v>43383</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -20669,50 +20376,87 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>83</v>
+    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F10" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" s="6"/>
+    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="F10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="F11" s="9" t="s">
-        <v>85</v>
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="F11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>87</v>
+    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="F12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -20724,26 +20468,240 @@
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="69" priority="7" operator="containsText" text="zablokowany">
-      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
+  <conditionalFormatting sqref="D1:D6">
+    <cfRule type="containsText" dxfId="69" priority="2" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="8" operator="containsText" text="pozytywny warunkowo">
-      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
+    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="9" operator="containsText" text="pozytywny">
-      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
+    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="10" operator="containsText" text="nieprzetestowano">
-      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
+    <cfRule type="containsText" dxfId="66" priority="5" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="65" priority="6" operator="containsText" text="negatywny">
-      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
+  <conditionalFormatting sqref="D1:D6">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D5">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9741D50-4AEE-45D3-BFC6-BF01A15F6C84}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7">
+        <v>43383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="F12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:D6">
     <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="zablokowany">
       <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
     </cfRule>
@@ -20757,7 +20715,7 @@
       <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D5">
+  <conditionalFormatting sqref="D1:D6">
     <cfRule type="containsText" dxfId="60" priority="1" operator="containsText" text="negatywny">
       <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
     </cfRule>
@@ -20766,25 +20724,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770724BE-A242-4B78-9330-98FF62807E0C}">
-  <dimension ref="A1:K13"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1201DBF-776F-4E80-B326-18F6F5DF3A00}">
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -20846,7 +20804,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7">
-        <v>43388</v>
+        <v>43387</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -20884,53 +20842,76 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="255" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>93</v>
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="F10" s="9" t="s">
-        <v>96</v>
+        <v>76</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="F11" s="9" t="s">
-        <v>74</v>
+        <v>85</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
-        <v>98</v>
+    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="F12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -20982,4 +20963,258 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770724BE-A242-4B78-9330-98FF62807E0C}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7">
+        <v>43388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="F10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="F11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="F12" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="F13" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="49" priority="7" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="8" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="9" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="45" priority="6" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>